<commit_message>
Test to see if getting data from excel sheet
</commit_message>
<xml_diff>
--- a/tests/data_testfile.xlsx
+++ b/tests/data_testfile.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natea\PycharmProjects\NateAnderson_Project1Sprint1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BEE758A2-55D1-4D04-BACC-264EC11C4B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFED059F-AC63-4AEB-B58F-E567C6E8B05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33645" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{9EA79192-EBC7-45B3-81F3-54D6F8B482D1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="State_M2019_dl" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>